<commit_message>
EPBDS-11051 Test is added
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA1F13-72A1-4C09-9CBE-17F37426B06A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
+    <workbookView xWindow="3760" yWindow="2770" windowWidth="23750" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>return java.lang.Boolean.TRUE;</t>
   </si>
@@ -38,12 +44,33 @@
   </si>
   <si>
     <t>Test test2</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult  mapSpr(String a, Map bMap, String java)</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>= java.lang.String.class</t>
+  </si>
+  <si>
+    <t>= java.lang.Boolean.TRUE;</t>
+  </si>
+  <si>
+    <t>step1</t>
+  </si>
+  <si>
+    <t>step2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -66,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -74,45 +101,30 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -465,80 +477,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="b">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D10" s="3" t="b">
+      <c r="D10" s="1" t="b">
         <v>1</v>
       </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-11051 Improve performance in OpenLClassLoader usage
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA1F13-72A1-4C09-9CBE-17F37426B06A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159775EC-3615-409C-823A-E2C2D9575EF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="2770" windowWidth="23750" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12940" yWindow="3130" windowWidth="23750" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>return java.lang.Boolean.TRUE;</t>
   </si>
@@ -44,27 +44,6 @@
   </si>
   <si>
     <t>Test test2</t>
-  </si>
-  <si>
-    <t>Spreadsheet SpreadsheetResult  mapSpr(String a, Map bMap, String java)</t>
-  </si>
-  <si>
-    <t>Steps</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>= java.lang.String.class</t>
-  </si>
-  <si>
-    <t>= java.lang.Boolean.TRUE;</t>
-  </si>
-  <si>
-    <t>step1</t>
-  </si>
-  <si>
-    <t>step2</t>
   </si>
 </sst>
 </file>
@@ -481,7 +460,7 @@
   <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -566,9 +545,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18"/>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
+      <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
@@ -577,12 +554,8 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19"/>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
+      <c r="B19"/>
+      <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
@@ -590,12 +563,8 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20"/>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B20"/>
+      <c r="C20" s="2"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -603,12 +572,8 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21"/>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B21"/>
+      <c r="C21" s="2"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>

</xml_diff>

<commit_message>
EPBDS-11051 Fix local variables visibility bug on full class name analyze algoritm
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159775EC-3615-409C-823A-E2C2D9575EF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DB63B5-C768-4545-9105-7226A6CD1E75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12940" yWindow="3130" windowWidth="23750" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18030" yWindow="3130" windowWidth="18660" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>return java.lang.Boolean.TRUE;</t>
   </si>
@@ -44,6 +44,51 @@
   </si>
   <si>
     <t>Test test2</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult calc()</t>
+  </si>
+  <si>
+    <t>Step Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Step1</t>
+  </si>
+  <si>
+    <t>Step2</t>
+  </si>
+  <si>
+    <t>Step3</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>Step5</t>
+  </si>
+  <si>
+    <t>= for (int java=0;java&lt;10;java++) {} java.lang.Boolean.TRUE;</t>
+  </si>
+  <si>
+    <t>= for (int i=0;i&lt;10;i++) { String java = "hello";} java.lang.Boolean.TRUE;</t>
+  </si>
+  <si>
+    <t>= if (true) {String java = "Hello";} java.lang.Boolean.TRUE;</t>
+  </si>
+  <si>
+    <t>= while (false) {String java = "Hello";} java.lang.Boolean.TRUE;</t>
+  </si>
+  <si>
+    <t>= {String java = "Hello";} java.lang.Boolean.TRUE;</t>
+  </si>
+  <si>
+    <t>Step6</t>
+  </si>
+  <si>
+    <t>while (</t>
   </si>
 </sst>
 </file>
@@ -457,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:G21"/>
+  <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -525,10 +570,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
@@ -536,8 +590,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
@@ -545,8 +603,12 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -554,8 +616,12 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
@@ -563,8 +629,12 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -572,12 +642,24 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
EPBDS-11051 Revert the fix local variables visibility bug on full class name analyze algoritm
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/FullJavaClassName.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DB63B5-C768-4545-9105-7226A6CD1E75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C6A0E7-CC0D-4740-AA6C-38B804360F9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18030" yWindow="3130" windowWidth="18660" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>return java.lang.Boolean.TRUE;</t>
   </si>
@@ -44,51 +44,6 @@
   </si>
   <si>
     <t>Test test2</t>
-  </si>
-  <si>
-    <t>Spreadsheet SpreadsheetResult calc()</t>
-  </si>
-  <si>
-    <t>Step Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Step1</t>
-  </si>
-  <si>
-    <t>Step2</t>
-  </si>
-  <si>
-    <t>Step3</t>
-  </si>
-  <si>
-    <t>Step4</t>
-  </si>
-  <si>
-    <t>Step5</t>
-  </si>
-  <si>
-    <t>= for (int java=0;java&lt;10;java++) {} java.lang.Boolean.TRUE;</t>
-  </si>
-  <si>
-    <t>= for (int i=0;i&lt;10;i++) { String java = "hello";} java.lang.Boolean.TRUE;</t>
-  </si>
-  <si>
-    <t>= if (true) {String java = "Hello";} java.lang.Boolean.TRUE;</t>
-  </si>
-  <si>
-    <t>= while (false) {String java = "Hello";} java.lang.Boolean.TRUE;</t>
-  </si>
-  <si>
-    <t>= {String java = "Hello";} java.lang.Boolean.TRUE;</t>
-  </si>
-  <si>
-    <t>Step6</t>
-  </si>
-  <si>
-    <t>while (</t>
   </si>
 </sst>
 </file>
@@ -505,7 +460,7 @@
   <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A15" sqref="A15:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -570,19 +525,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16"/>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
+      <c r="B16"/>
+      <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
@@ -590,12 +536,8 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17"/>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="B17"/>
+      <c r="C17" s="2"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
@@ -603,12 +545,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18"/>
-      <c r="B18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C18" s="2"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -616,12 +553,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19"/>
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C19" s="2"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
@@ -629,12 +561,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20"/>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -642,24 +569,14 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21"/>
-      <c r="B21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="C21" s="2"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C22" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>